<commit_message>
Amendments following checks by YH
</commit_message>
<xml_diff>
--- a/data/processed/202308-services-list-processed-final.xlsx
+++ b/data/processed/202308-services-list-processed-final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Desktop\Turing\Projects\decision-services-index\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{317B8BC4-FCFB-45A2-8AFB-2FFC9D92125B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFA46CA-C957-4E12-8ACE-DDB221E20F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1635" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="17460" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4448" uniqueCount="1161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4449" uniqueCount="1163">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -3164,9 +3164,6 @@
     <t>Check driving information appears on the Web Archive page. 17,606, 215</t>
   </si>
   <si>
-    <t>From web archive: 659,734,690</t>
-  </si>
-  <si>
     <t>web_archive_value</t>
   </si>
   <si>
@@ -3275,9 +3272,6 @@
     <t>Carer's allowance new claims</t>
   </si>
   <si>
-    <t>New ESA claims as per this website: https://www.gov.uk/government/statistics/dwp-benefits-statistics-august-2023/dwp-benefits-statistics-august-2023</t>
-  </si>
-  <si>
     <t>other_website_value</t>
   </si>
   <si>
@@ -3519,6 +3513,18 @@
   </si>
   <si>
     <t>final_transactions_value_source</t>
+  </si>
+  <si>
+    <t>23,000 initial WCAs per quarter reported in most recent data release here https://www.gov.uk/government/statistics/esa-outcomes-of-work-capability-assessments-including-mandatory-reconsiderations-and-appeals-december-2023/esa-outcomes-of-work-capability-assessments-including-mandatory-reconsiderations-and-appeals-december-2023</t>
+  </si>
+  <si>
+    <t>We have used the number for new claims rather than existing claims</t>
+  </si>
+  <si>
+    <t>present on the website but no data. This value is the most recent (non-digital) historic figure</t>
+  </si>
+  <si>
+    <t>From web archive: 659,734,690 (vehicle tax: checks by individuals)</t>
   </si>
 </sst>
 </file>
@@ -3905,10 +3911,10 @@
   <dimension ref="A1:Y378"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -3942,19 +3948,19 @@
         <v>1036</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
@@ -4022,7 +4028,7 @@
         <v>1037</v>
       </c>
       <c r="I2" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K2">
         <v>101483774</v>
@@ -4080,10 +4086,10 @@
         <v>1425606</v>
       </c>
       <c r="I3" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="K3">
         <v>89356303</v>
@@ -4136,10 +4142,10 @@
         <v>1037</v>
       </c>
       <c r="I4" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J4" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="K4">
         <v>43647011</v>
@@ -4192,10 +4198,10 @@
         <v>7774</v>
       </c>
       <c r="I5" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J5" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="K5">
         <v>31316079</v>
@@ -4249,7 +4255,7 @@
         <v>47055169</v>
       </c>
       <c r="I6" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="K6">
         <v>28787010</v>
@@ -4302,7 +4308,7 @@
         <v>1037</v>
       </c>
       <c r="I7" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K7">
         <v>28197611</v>
@@ -4359,10 +4365,10 @@
         <v>659734690</v>
       </c>
       <c r="I8" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J8" t="s">
-        <v>1042</v>
+        <v>1162</v>
       </c>
       <c r="K8">
         <v>26027161</v>
@@ -4415,7 +4421,7 @@
         <v>1037</v>
       </c>
       <c r="I9" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K9">
         <v>22211549</v>
@@ -4468,10 +4474,10 @@
         <v>1037</v>
       </c>
       <c r="I10" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J10" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="K10">
         <v>13095804</v>
@@ -4529,10 +4535,10 @@
         <v>6926256</v>
       </c>
       <c r="I11" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J11" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="K11">
         <v>12806975</v>
@@ -4585,10 +4591,10 @@
         <v>1037</v>
       </c>
       <c r="I12" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J12" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="K12">
         <v>9117063</v>
@@ -4641,7 +4647,7 @@
         <v>1037</v>
       </c>
       <c r="I13" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K13">
         <v>7664212</v>
@@ -4700,10 +4706,10 @@
         <v>38225014</v>
       </c>
       <c r="I14" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J14" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="K14">
         <v>6852544</v>
@@ -4756,7 +4762,7 @@
         <v>1037</v>
       </c>
       <c r="I15" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K15">
         <v>6565740</v>
@@ -4809,10 +4815,10 @@
         <v>1037</v>
       </c>
       <c r="I16" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J16" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K16">
         <v>5954359</v>
@@ -4868,10 +4874,10 @@
         <v>34175</v>
       </c>
       <c r="I17" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J17" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="K17">
         <v>5108079</v>
@@ -4924,10 +4930,10 @@
         <v>30112</v>
       </c>
       <c r="I18" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J18" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="K18">
         <v>4341278</v>
@@ -4980,10 +4986,10 @@
         <v>3515162</v>
       </c>
       <c r="I19" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J19" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="K19">
         <v>3432014</v>
@@ -5039,10 +5045,10 @@
         <v>1037</v>
       </c>
       <c r="I20" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J20" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="K20">
         <v>3430180</v>
@@ -5095,7 +5101,7 @@
         <v>1037</v>
       </c>
       <c r="I21" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K21">
         <v>3387429</v>
@@ -5151,10 +5157,10 @@
         <v>1037</v>
       </c>
       <c r="I22" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J22" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K22">
         <v>2832843</v>
@@ -5208,7 +5214,7 @@
         <v>3793771</v>
       </c>
       <c r="I23" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="K23">
         <v>2762294</v>
@@ -5261,7 +5267,7 @@
         <v>1037</v>
       </c>
       <c r="I24" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K24">
         <v>2700716</v>
@@ -5315,7 +5321,7 @@
         <v>1122022</v>
       </c>
       <c r="I25" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="K25">
         <v>2544197</v>
@@ -5368,7 +5374,7 @@
         <v>1037</v>
       </c>
       <c r="I26" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K26">
         <v>2496953</v>
@@ -5428,10 +5434,10 @@
         <v>594119</v>
       </c>
       <c r="I27" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J27" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="K27">
         <v>2375312</v>
@@ -5484,7 +5490,7 @@
         <v>1037</v>
       </c>
       <c r="I28" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K28">
         <v>2373627</v>
@@ -5537,10 +5543,10 @@
         <v>650002</v>
       </c>
       <c r="I29" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J29" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="K29">
         <v>2318856</v>
@@ -5584,10 +5590,10 @@
         <v>510</v>
       </c>
       <c r="D30" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="E30" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="F30" t="s">
         <v>1037</v>
@@ -5596,10 +5602,10 @@
         <v>1633731</v>
       </c>
       <c r="I30" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J30" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="K30">
         <v>2208842</v>
@@ -5656,7 +5662,7 @@
         <v>10382205</v>
       </c>
       <c r="I31" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="K31">
         <v>1798004</v>
@@ -5709,10 +5715,10 @@
         <v>1037</v>
       </c>
       <c r="I32" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J32" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="K32">
         <v>1779596</v>
@@ -5765,7 +5771,7 @@
         <v>1037</v>
       </c>
       <c r="I33" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K33">
         <v>1710581</v>
@@ -5824,10 +5830,10 @@
         <v>1037</v>
       </c>
       <c r="I34" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J34" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="K34">
         <v>1678413</v>
@@ -5883,10 +5889,10 @@
         <v>1327057</v>
       </c>
       <c r="I35" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J35" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="K35">
         <v>1608817</v>
@@ -5939,10 +5945,10 @@
         <v>1037</v>
       </c>
       <c r="I36" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J36" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K36">
         <v>1476035</v>
@@ -6007,7 +6013,7 @@
         <v>17606215</v>
       </c>
       <c r="I37" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J37" t="s">
         <v>1041</v>
@@ -6067,7 +6073,7 @@
         <v>1480669</v>
       </c>
       <c r="I38" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="K38">
         <v>1368538</v>
@@ -6120,10 +6126,10 @@
         <v>1037</v>
       </c>
       <c r="I39" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J39" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="K39">
         <v>1269369</v>
@@ -6176,10 +6182,10 @@
         <v>1037</v>
       </c>
       <c r="I40" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J40" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="K40">
         <v>1245607</v>
@@ -6236,7 +6242,7 @@
         <v>2336377</v>
       </c>
       <c r="I41" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="K41">
         <v>1209557</v>
@@ -6292,7 +6298,7 @@
         <v>1430186</v>
       </c>
       <c r="I42" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="K42">
         <v>1144686</v>
@@ -6345,7 +6351,7 @@
         <v>1037</v>
       </c>
       <c r="I43" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K43">
         <v>1103739</v>
@@ -6398,7 +6404,7 @@
         <v>1037</v>
       </c>
       <c r="I44" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K44">
         <v>1054826</v>
@@ -6463,7 +6469,7 @@
         <v>1037</v>
       </c>
       <c r="I45" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K45">
         <v>1019495</v>
@@ -6519,7 +6525,7 @@
         <v>1037</v>
       </c>
       <c r="I46" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K46">
         <v>1019041</v>
@@ -6584,10 +6590,10 @@
         <v>3921728</v>
       </c>
       <c r="I47" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J47" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="K47">
         <v>1012591</v>
@@ -6640,7 +6646,7 @@
         <v>1037</v>
       </c>
       <c r="I48" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K48">
         <v>931824</v>
@@ -6693,7 +6699,7 @@
         <v>1037</v>
       </c>
       <c r="I49" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K49">
         <v>908702</v>
@@ -6746,10 +6752,10 @@
         <v>1037</v>
       </c>
       <c r="I50" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J50" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K50">
         <v>784779</v>
@@ -6802,13 +6808,16 @@
         <v>1018</v>
       </c>
       <c r="F51" s="2">
-        <v>12896460</v>
+        <v>434682</v>
       </c>
       <c r="H51" s="2">
-        <v>12896460</v>
+        <v>434682</v>
       </c>
       <c r="I51" t="s">
-        <v>1149</v>
+        <v>1147</v>
+      </c>
+      <c r="J51" t="s">
+        <v>1160</v>
       </c>
       <c r="K51">
         <v>731350</v>
@@ -6861,10 +6870,10 @@
         <v>1037</v>
       </c>
       <c r="I52" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J52" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K52">
         <v>700674</v>
@@ -6917,7 +6926,7 @@
         <v>1037</v>
       </c>
       <c r="I53" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K53">
         <v>688969</v>
@@ -6975,10 +6984,10 @@
         <v>1404024</v>
       </c>
       <c r="I54" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J54" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="K54">
         <v>647916</v>
@@ -7031,7 +7040,7 @@
         <v>1037</v>
       </c>
       <c r="I55" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K55">
         <v>616708</v>
@@ -7087,7 +7096,7 @@
         <v>1164471</v>
       </c>
       <c r="I56" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="K56">
         <v>592600</v>
@@ -7140,7 +7149,7 @@
         <v>1037</v>
       </c>
       <c r="I57" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K57">
         <v>584286</v>
@@ -7205,7 +7214,7 @@
         <v>1037</v>
       </c>
       <c r="I58" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K58">
         <v>551396</v>
@@ -7258,7 +7267,7 @@
         <v>1037</v>
       </c>
       <c r="I59" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K59">
         <v>550011</v>
@@ -7311,7 +7320,7 @@
         <v>1037</v>
       </c>
       <c r="I60" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K60">
         <v>540419</v>
@@ -7364,7 +7373,7 @@
         <v>1037</v>
       </c>
       <c r="I61" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K61">
         <v>528352</v>
@@ -7417,10 +7426,10 @@
         <v>1037</v>
       </c>
       <c r="I62" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J62" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="K62">
         <v>527319</v>
@@ -7477,10 +7486,10 @@
         <v>594119</v>
       </c>
       <c r="I63" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J63" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="K63">
         <v>476540</v>
@@ -7533,10 +7542,10 @@
         <v>282303</v>
       </c>
       <c r="I64" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J64" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="K64">
         <v>443305</v>
@@ -7589,10 +7598,10 @@
         <v>1037</v>
       </c>
       <c r="I65" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J65" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="K65">
         <v>440167</v>
@@ -7647,10 +7656,10 @@
         <v>492972</v>
       </c>
       <c r="I66" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J66" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="K66">
         <v>437515</v>
@@ -7706,10 +7715,10 @@
         <v>1900000</v>
       </c>
       <c r="I67" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J67" t="s">
-        <v>1101</v>
+        <v>1161</v>
       </c>
       <c r="K67">
         <v>433472</v>
@@ -7762,10 +7771,10 @@
         <v>1037</v>
       </c>
       <c r="I68" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J68" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="K68">
         <v>431284</v>
@@ -7818,10 +7827,10 @@
         <v>1037</v>
       </c>
       <c r="I69" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J69" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="K69">
         <v>429725</v>
@@ -7874,10 +7883,10 @@
         <v>1037</v>
       </c>
       <c r="I70" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J70" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K70">
         <v>414018</v>
@@ -7930,10 +7939,10 @@
         <v>1037</v>
       </c>
       <c r="I71" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J71" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K71">
         <v>402173</v>
@@ -7986,7 +7995,7 @@
         <v>1037</v>
       </c>
       <c r="I72" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K72">
         <v>398533</v>
@@ -8042,7 +8051,7 @@
         <v>1037</v>
       </c>
       <c r="I73" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K73">
         <v>368490</v>
@@ -8095,10 +8104,10 @@
         <v>1037</v>
       </c>
       <c r="I74" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J74" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="K74">
         <v>360298</v>
@@ -8163,7 +8172,7 @@
         <v>1037</v>
       </c>
       <c r="I75" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K75">
         <v>351337</v>
@@ -8219,10 +8228,10 @@
         <v>114097</v>
       </c>
       <c r="I76" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J76" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="K76">
         <v>339123</v>
@@ -8275,10 +8284,10 @@
         <v>1037</v>
       </c>
       <c r="I77" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J77" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K77">
         <v>327256</v>
@@ -8343,7 +8352,7 @@
         <v>1037</v>
       </c>
       <c r="I78" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K78">
         <v>326786</v>
@@ -8402,10 +8411,10 @@
         <v>200789</v>
       </c>
       <c r="I79" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J79" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="K79">
         <v>317453</v>
@@ -8458,7 +8467,7 @@
         <v>1037</v>
       </c>
       <c r="I80" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K80">
         <v>302402</v>
@@ -8514,7 +8523,7 @@
         <v>1037</v>
       </c>
       <c r="I81" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K81">
         <v>301136</v>
@@ -8567,16 +8576,17 @@
         <v>1037</v>
       </c>
       <c r="G82">
-        <v>97000</v>
+        <f>23000*4</f>
+        <v>92000</v>
       </c>
       <c r="H82">
-        <v>97000</v>
+        <v>92000</v>
       </c>
       <c r="I82" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="J82" t="s">
-        <v>1079</v>
+        <v>1159</v>
       </c>
       <c r="K82">
         <v>282295</v>
@@ -8629,10 +8639,10 @@
         <v>1037</v>
       </c>
       <c r="I83" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J83" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="K83">
         <v>264322</v>
@@ -8689,10 +8699,10 @@
         <v>594119</v>
       </c>
       <c r="I84" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J84" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="K84">
         <v>262579</v>
@@ -8748,7 +8758,7 @@
         <v>98417</v>
       </c>
       <c r="I85" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="K85">
         <v>262129</v>
@@ -8792,7 +8802,7 @@
         <v>769</v>
       </c>
       <c r="E86" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="F86" t="s">
         <v>1037</v>
@@ -8801,10 +8811,10 @@
         <v>482309</v>
       </c>
       <c r="I86" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J86" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="K86">
         <v>253487</v>
@@ -8862,10 +8872,10 @@
         <v>29783.5</v>
       </c>
       <c r="I87" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J87" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="K87">
         <v>244851</v>
@@ -8918,7 +8928,7 @@
         <v>1037</v>
       </c>
       <c r="I88" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K88">
         <v>244793</v>
@@ -8971,7 +8981,7 @@
         <v>1037</v>
       </c>
       <c r="I89" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K89">
         <v>240842</v>
@@ -9024,7 +9034,7 @@
         <v>1037</v>
       </c>
       <c r="I90" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K90">
         <v>233418</v>
@@ -9077,7 +9087,7 @@
         <v>1037</v>
       </c>
       <c r="I91" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K91">
         <v>224072</v>
@@ -9142,10 +9152,10 @@
         <v>1037</v>
       </c>
       <c r="I92" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J92" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="K92">
         <v>220282</v>
@@ -9201,10 +9211,10 @@
         <v>1037</v>
       </c>
       <c r="I93" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J93" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="K93">
         <v>205056</v>
@@ -9257,10 +9267,10 @@
         <v>1037</v>
       </c>
       <c r="I94" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J94" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="K94">
         <v>193213</v>
@@ -9316,10 +9326,10 @@
         <v>280673</v>
       </c>
       <c r="I95" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J95" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="K95">
         <v>184716</v>
@@ -9372,10 +9382,10 @@
         <v>228622</v>
       </c>
       <c r="I96" t="s">
+        <v>1149</v>
+      </c>
+      <c r="J96" t="s">
         <v>1151</v>
-      </c>
-      <c r="J96" t="s">
-        <v>1153</v>
       </c>
       <c r="K96">
         <v>166877</v>
@@ -9430,10 +9440,10 @@
         <v>173691</v>
       </c>
       <c r="I97" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J97" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="K97">
         <v>157677</v>
@@ -9487,10 +9497,10 @@
         <v>150773</v>
       </c>
       <c r="I98" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J98" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="K98">
         <v>157031</v>
@@ -9543,10 +9553,10 @@
         <v>472797</v>
       </c>
       <c r="I99" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J99" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="K99">
         <v>153514</v>
@@ -9599,10 +9609,10 @@
         <v>1037</v>
       </c>
       <c r="I100" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J100" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="K100">
         <v>150912</v>
@@ -9655,7 +9665,7 @@
         <v>1037</v>
       </c>
       <c r="I101" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K101">
         <v>150912</v>
@@ -9708,10 +9718,10 @@
         <v>1037</v>
       </c>
       <c r="I102" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J102" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K102">
         <v>149790</v>
@@ -9764,7 +9774,7 @@
         <v>1037</v>
       </c>
       <c r="I103" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K103">
         <v>148961</v>
@@ -9829,7 +9839,7 @@
         <v>1037</v>
       </c>
       <c r="I104" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K104">
         <v>147743</v>
@@ -9885,7 +9895,7 @@
         <v>282303</v>
       </c>
       <c r="I105" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="K105">
         <v>147133</v>
@@ -9938,10 +9948,10 @@
         <v>1037</v>
       </c>
       <c r="I106" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J106" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K106">
         <v>137895</v>
@@ -9997,10 +10007,10 @@
         <v>1037</v>
       </c>
       <c r="I107" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J107" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="K107">
         <v>129028</v>
@@ -10053,10 +10063,10 @@
         <v>959421</v>
       </c>
       <c r="I108" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J108" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="K108">
         <v>126038</v>
@@ -10112,10 +10122,10 @@
         <v>30112</v>
       </c>
       <c r="I109" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J109" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="K109">
         <v>124017</v>
@@ -10168,10 +10178,10 @@
         <v>1037</v>
       </c>
       <c r="I110" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J110" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="K110">
         <v>121743</v>
@@ -10224,10 +10234,10 @@
         <v>1037</v>
       </c>
       <c r="I111" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J111" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="K111">
         <v>113309</v>
@@ -10280,10 +10290,10 @@
         <v>1037</v>
       </c>
       <c r="I112" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J112" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K112">
         <v>112708</v>
@@ -10339,7 +10349,7 @@
         <v>1037</v>
       </c>
       <c r="I113" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K113">
         <v>109350</v>
@@ -10392,7 +10402,7 @@
         <v>1037</v>
       </c>
       <c r="I114" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K114">
         <v>108633</v>
@@ -10436,7 +10446,7 @@
         <v>710</v>
       </c>
       <c r="E115" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="F115" t="s">
         <v>1037</v>
@@ -10446,10 +10456,10 @@
         <v>1292118</v>
       </c>
       <c r="I115" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J115" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="K115">
         <v>105936</v>
@@ -10514,7 +10524,7 @@
         <v>1037</v>
       </c>
       <c r="I116" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K116">
         <v>93399</v>
@@ -10570,10 +10580,10 @@
         <v>1517654</v>
       </c>
       <c r="I117" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J117" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="K117">
         <v>87117</v>
@@ -10629,10 +10639,10 @@
         <v>1037</v>
       </c>
       <c r="I118" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J118" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="K118">
         <v>83957</v>
@@ -10685,10 +10695,10 @@
         <v>1037</v>
       </c>
       <c r="I119" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J119" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K119">
         <v>70951</v>
@@ -10741,7 +10751,7 @@
         <v>1037</v>
       </c>
       <c r="I120" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K120">
         <v>70661</v>
@@ -10794,7 +10804,7 @@
         <v>1037</v>
       </c>
       <c r="I121" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K121">
         <v>70188</v>
@@ -10838,7 +10848,7 @@
         <v>535</v>
       </c>
       <c r="E122" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="F122" t="s">
         <v>1037</v>
@@ -10847,10 +10857,10 @@
         <v>155823</v>
       </c>
       <c r="I122" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J122" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="K122">
         <v>66885</v>
@@ -10903,10 +10913,10 @@
         <v>64274</v>
       </c>
       <c r="I123" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J123" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="K123">
         <v>63149</v>
@@ -10959,10 +10969,10 @@
         <v>1593</v>
       </c>
       <c r="I124" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J124" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="K124">
         <v>61304</v>
@@ -11015,7 +11025,7 @@
         <v>1037</v>
       </c>
       <c r="I125" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K125">
         <v>61159</v>
@@ -11068,10 +11078,10 @@
         <v>91874</v>
       </c>
       <c r="I126" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J126" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="K126">
         <v>61106</v>
@@ -11124,10 +11134,10 @@
         <v>1037</v>
       </c>
       <c r="I127" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J127" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="K127">
         <v>60892</v>
@@ -11180,7 +11190,7 @@
         <v>1037</v>
       </c>
       <c r="I128" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K128">
         <v>60347</v>
@@ -11239,10 +11249,10 @@
         <v>37710</v>
       </c>
       <c r="I129" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="J129" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="K129">
         <v>59478</v>
@@ -11295,10 +11305,10 @@
         <v>58220</v>
       </c>
       <c r="I130" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J130" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="K130">
         <v>57316</v>
@@ -11351,7 +11361,7 @@
         <v>1037</v>
       </c>
       <c r="I131" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K131">
         <v>57128</v>
@@ -11416,10 +11426,10 @@
         <v>1037</v>
       </c>
       <c r="I132" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J132" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K132">
         <v>53417</v>
@@ -11475,10 +11485,10 @@
         <v>42000</v>
       </c>
       <c r="I133" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J133" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="K133">
         <v>49588</v>
@@ -11531,10 +11541,10 @@
         <v>1037</v>
       </c>
       <c r="I134" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J134" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="K134">
         <v>47735</v>
@@ -11595,10 +11605,10 @@
         <v>488096</v>
       </c>
       <c r="I135" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J135" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="K135">
         <v>46152</v>
@@ -11654,10 +11664,10 @@
         <v>444119</v>
       </c>
       <c r="I136" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J136" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="K136">
         <v>43816</v>
@@ -11710,10 +11720,10 @@
         <v>1037</v>
       </c>
       <c r="I137" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J137" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K137">
         <v>42414</v>
@@ -11769,10 +11779,10 @@
         <v>19601</v>
       </c>
       <c r="I138" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J138" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="K138">
         <v>39764</v>
@@ -11825,10 +11835,10 @@
         <v>1037</v>
       </c>
       <c r="I139" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J139" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="K139">
         <v>39122</v>
@@ -11881,10 +11891,10 @@
         <v>32787</v>
       </c>
       <c r="I140" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J140" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="K140">
         <v>39061</v>
@@ -11941,10 +11951,10 @@
         <v>902186</v>
       </c>
       <c r="I141" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J141" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="K141">
         <v>39004</v>
@@ -11997,10 +12007,10 @@
         <v>1037</v>
       </c>
       <c r="I142" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J142" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="K142">
         <v>35848</v>
@@ -12056,7 +12066,7 @@
         <v>1037</v>
       </c>
       <c r="I143" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K143">
         <v>34990</v>
@@ -12109,7 +12119,7 @@
         <v>1037</v>
       </c>
       <c r="I144" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K144">
         <v>34757</v>
@@ -12165,7 +12175,7 @@
         <v>1037</v>
       </c>
       <c r="I145" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K145">
         <v>33894</v>
@@ -12218,7 +12228,7 @@
         <v>1037</v>
       </c>
       <c r="I146" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K146">
         <v>33456</v>
@@ -12271,7 +12281,7 @@
         <v>1037</v>
       </c>
       <c r="I147" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K147">
         <v>32332</v>
@@ -12324,7 +12334,7 @@
         <v>1037</v>
       </c>
       <c r="I148" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K148">
         <v>31908</v>
@@ -12377,10 +12387,10 @@
         <v>1037</v>
       </c>
       <c r="I149" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J149" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K149">
         <v>31571</v>
@@ -12436,10 +12446,10 @@
         <v>1037</v>
       </c>
       <c r="I150" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J150" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K150">
         <v>30447</v>
@@ -12495,10 +12505,10 @@
         <v>182588</v>
       </c>
       <c r="I151" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J151" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="K151">
         <v>30377</v>
@@ -12551,10 +12561,10 @@
         <v>11778</v>
       </c>
       <c r="I152" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J152" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="K152">
         <v>29530</v>
@@ -12607,7 +12617,7 @@
         <v>1037</v>
       </c>
       <c r="I153" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K153">
         <v>25460</v>
@@ -12660,7 +12670,7 @@
         <v>1037</v>
       </c>
       <c r="I154" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K154">
         <v>25075</v>
@@ -12713,7 +12723,7 @@
         <v>1037</v>
       </c>
       <c r="I155" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K155">
         <v>23694</v>
@@ -12769,10 +12779,10 @@
         <v>1037</v>
       </c>
       <c r="I156" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J156" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="K156">
         <v>22986</v>
@@ -12829,10 +12839,10 @@
         <v>8631</v>
       </c>
       <c r="I157" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J157" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="K157">
         <v>22514</v>
@@ -12885,10 +12895,10 @@
         <v>1037</v>
       </c>
       <c r="I158" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J158" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K158">
         <v>22413</v>
@@ -12941,10 +12951,10 @@
         <v>1037</v>
       </c>
       <c r="I159" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J159" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K159">
         <v>22172</v>
@@ -12997,10 +13007,10 @@
         <v>1037</v>
       </c>
       <c r="I160" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J160" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K160">
         <v>22172</v>
@@ -13058,10 +13068,10 @@
         <v>29783.5</v>
       </c>
       <c r="I161" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J161" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="K161">
         <v>21897</v>
@@ -13114,10 +13124,10 @@
         <v>1037</v>
       </c>
       <c r="I162" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J162" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K162">
         <v>20929</v>
@@ -13170,7 +13180,7 @@
         <v>1037</v>
       </c>
       <c r="I163" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K163">
         <v>20917</v>
@@ -13238,10 +13248,10 @@
         <v>1037</v>
       </c>
       <c r="I164" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J164" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="K164">
         <v>20724</v>
@@ -13294,10 +13304,10 @@
         <v>1037</v>
       </c>
       <c r="I165" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J165" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="K165">
         <v>20693</v>
@@ -13350,10 +13360,10 @@
         <v>1037</v>
       </c>
       <c r="I166" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J166" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K166">
         <v>19588</v>
@@ -13412,10 +13422,10 @@
         <v>1037</v>
       </c>
       <c r="I167" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J167" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="K167">
         <v>19493</v>
@@ -13468,7 +13478,7 @@
         <v>1037</v>
       </c>
       <c r="I168" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K168">
         <v>19266</v>
@@ -13521,7 +13531,7 @@
         <v>1037</v>
       </c>
       <c r="I169" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K169">
         <v>18692</v>
@@ -13577,10 +13587,10 @@
         <v>64507</v>
       </c>
       <c r="I170" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J170" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="K170">
         <v>18563</v>
@@ -13636,7 +13646,7 @@
         <v>17766</v>
       </c>
       <c r="I171" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="K171">
         <v>18299</v>
@@ -13689,7 +13699,7 @@
         <v>1037</v>
       </c>
       <c r="I172" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K172">
         <v>17311</v>
@@ -13745,10 +13755,10 @@
         <v>1037</v>
       </c>
       <c r="I173" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J173" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K173">
         <v>17086</v>
@@ -13801,10 +13811,10 @@
         <v>1037</v>
       </c>
       <c r="I174" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J174" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="K174">
         <v>16241</v>
@@ -13857,7 +13867,7 @@
         <v>1037</v>
       </c>
       <c r="I175" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K175">
         <v>16165</v>
@@ -13910,10 +13920,10 @@
         <v>1037</v>
       </c>
       <c r="I176" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J176" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K176">
         <v>16092</v>
@@ -13966,7 +13976,7 @@
         <v>1037</v>
       </c>
       <c r="I177" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K177">
         <v>15800</v>
@@ -14019,7 +14029,7 @@
         <v>1037</v>
       </c>
       <c r="I178" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K178">
         <v>15798</v>
@@ -14072,7 +14082,7 @@
         <v>1037</v>
       </c>
       <c r="I179" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K179">
         <v>15088</v>
@@ -14140,10 +14150,10 @@
         <v>43760</v>
       </c>
       <c r="I180" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="J180" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="K180">
         <v>15031</v>
@@ -14196,10 +14206,10 @@
         <v>1037</v>
       </c>
       <c r="I181" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J181" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K181">
         <v>14908</v>
@@ -14252,10 +14262,10 @@
         <v>1037</v>
       </c>
       <c r="I182" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J182" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="K182">
         <v>14577</v>
@@ -14308,10 +14318,10 @@
         <v>1037</v>
       </c>
       <c r="I183" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J183" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="K183">
         <v>14179</v>
@@ -14365,7 +14375,7 @@
         <v>2459253</v>
       </c>
       <c r="I184" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="K184">
         <v>14179</v>
@@ -14418,7 +14428,7 @@
         <v>1037</v>
       </c>
       <c r="I185" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K185">
         <v>14135</v>
@@ -14471,10 +14481,10 @@
         <v>1037</v>
       </c>
       <c r="I186" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J186" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="K186">
         <v>13935</v>
@@ -14527,7 +14537,7 @@
         <v>1037</v>
       </c>
       <c r="I187" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K187">
         <v>13193</v>
@@ -14580,10 +14590,10 @@
         <v>1037</v>
       </c>
       <c r="I188" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J188" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K188">
         <v>13192</v>
@@ -14636,10 +14646,10 @@
         <v>1037</v>
       </c>
       <c r="I189" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J189" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="K189">
         <v>13159</v>
@@ -14694,10 +14704,10 @@
         <v>24076</v>
       </c>
       <c r="I190" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J190" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="K190">
         <v>13107</v>
@@ -14750,10 +14760,10 @@
         <v>1037</v>
       </c>
       <c r="I191" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J191" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K191">
         <v>13064</v>
@@ -14807,7 +14817,7 @@
         <v>14947</v>
       </c>
       <c r="I192" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="K192">
         <v>12553</v>
@@ -14860,10 +14870,10 @@
         <v>1037</v>
       </c>
       <c r="I193" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J193" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K193">
         <v>12444</v>
@@ -14916,7 +14926,7 @@
         <v>1037</v>
       </c>
       <c r="I194" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K194">
         <v>11515</v>
@@ -14969,10 +14979,10 @@
         <v>1037</v>
       </c>
       <c r="I195" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J195" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K195">
         <v>11031</v>
@@ -15025,10 +15035,10 @@
         <v>15118</v>
       </c>
       <c r="I196" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J196" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="K196">
         <v>10985</v>
@@ -15081,10 +15091,10 @@
         <v>1037</v>
       </c>
       <c r="I197" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J197" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="K197">
         <v>10919</v>
@@ -15149,7 +15159,7 @@
         <v>1037</v>
       </c>
       <c r="I198" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K198">
         <v>10916</v>
@@ -15202,7 +15212,7 @@
         <v>1037</v>
       </c>
       <c r="I199" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K199">
         <v>10879</v>
@@ -15246,7 +15256,7 @@
         <v>153</v>
       </c>
       <c r="E200" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="F200" t="s">
         <v>1037</v>
@@ -15255,7 +15265,7 @@
         <v>2299</v>
       </c>
       <c r="I200" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="K200">
         <v>10675</v>
@@ -15323,10 +15333,10 @@
         <v>53028</v>
       </c>
       <c r="I201" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J201" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="K201">
         <v>10662</v>
@@ -15382,10 +15392,10 @@
         <v>1037</v>
       </c>
       <c r="I202" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J202" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="K202">
         <v>10221</v>
@@ -15441,7 +15451,7 @@
         <v>1037</v>
       </c>
       <c r="I203" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K203">
         <v>10153</v>
@@ -15497,7 +15507,7 @@
         <v>1037</v>
       </c>
       <c r="I204" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K204">
         <v>10114</v>
@@ -15553,7 +15563,7 @@
         <v>1037</v>
       </c>
       <c r="I205" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K205">
         <v>10062</v>
@@ -15606,7 +15616,7 @@
         <v>1037</v>
       </c>
       <c r="I206" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K206">
         <v>9938</v>
@@ -15659,10 +15669,10 @@
         <v>1037</v>
       </c>
       <c r="I207" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J207" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K207">
         <v>9888</v>
@@ -15718,10 +15728,10 @@
         <v>1037</v>
       </c>
       <c r="I208" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J208" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K208">
         <v>9848</v>
@@ -15777,7 +15787,7 @@
         <v>1037</v>
       </c>
       <c r="I209" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K209">
         <v>9820</v>
@@ -15833,7 +15843,7 @@
         <v>1037</v>
       </c>
       <c r="I210" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K210">
         <v>9591</v>
@@ -15886,7 +15896,7 @@
         <v>1037</v>
       </c>
       <c r="I211" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K211">
         <v>9170</v>
@@ -15939,10 +15949,10 @@
         <v>1037</v>
       </c>
       <c r="I212" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J212" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K212">
         <v>8947</v>
@@ -15995,10 +16005,10 @@
         <v>1037</v>
       </c>
       <c r="I213" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J213" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K213">
         <v>8405</v>
@@ -16051,10 +16061,10 @@
         <v>1037</v>
       </c>
       <c r="I214" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J214" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="K214">
         <v>8399</v>
@@ -16110,10 +16120,10 @@
         <v>1037</v>
       </c>
       <c r="I215" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J215" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K215">
         <v>8323</v>
@@ -16166,7 +16176,7 @@
         <v>1037</v>
       </c>
       <c r="I216" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K216">
         <v>8195</v>
@@ -16219,10 +16229,10 @@
         <v>1037</v>
       </c>
       <c r="I217" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J217" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="K217">
         <v>8183</v>
@@ -16278,10 +16288,10 @@
         <v>3792</v>
       </c>
       <c r="I218" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J218" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="K218">
         <v>7376</v>
@@ -16334,7 +16344,7 @@
         <v>1037</v>
       </c>
       <c r="I219" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K219">
         <v>7365</v>
@@ -16387,7 +16397,7 @@
         <v>1037</v>
       </c>
       <c r="I220" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K220">
         <v>7241</v>
@@ -16440,7 +16450,7 @@
         <v>1037</v>
       </c>
       <c r="I221" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K221">
         <v>7127</v>
@@ -16496,7 +16506,7 @@
         <v>1037</v>
       </c>
       <c r="I222" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K222">
         <v>7059</v>
@@ -16549,10 +16559,10 @@
         <v>1037</v>
       </c>
       <c r="I223" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J223" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K223">
         <v>6944</v>
@@ -16608,10 +16618,10 @@
         <v>1037</v>
       </c>
       <c r="I224" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J224" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K224">
         <v>6829</v>
@@ -16664,7 +16674,7 @@
         <v>1037</v>
       </c>
       <c r="I225" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K225">
         <v>6716</v>
@@ -16732,10 +16742,10 @@
         <v>3039</v>
       </c>
       <c r="I226" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J226" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="K226">
         <v>6716</v>
@@ -16788,10 +16798,10 @@
         <v>1037</v>
       </c>
       <c r="I227" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J227" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K227">
         <v>6508</v>
@@ -16847,10 +16857,10 @@
         <v>1037</v>
       </c>
       <c r="I228" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J228" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K228">
         <v>6452</v>
@@ -16903,10 +16913,10 @@
         <v>1037</v>
       </c>
       <c r="I229" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J229" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K229">
         <v>6248</v>
@@ -16962,10 +16972,10 @@
         <v>1037</v>
       </c>
       <c r="I230" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J230" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K230">
         <v>6232</v>
@@ -17021,7 +17031,7 @@
         <v>1037</v>
       </c>
       <c r="I231" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K231">
         <v>5988</v>
@@ -17074,7 +17084,7 @@
         <v>1037</v>
       </c>
       <c r="I232" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K232">
         <v>5882</v>
@@ -17124,7 +17134,7 @@
         <v>313</v>
       </c>
       <c r="E233" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="F233" t="s">
         <v>1037</v>
@@ -17133,10 +17143,10 @@
         <v>64593</v>
       </c>
       <c r="I233" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J233" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="K233">
         <v>5748</v>
@@ -17189,7 +17199,7 @@
         <v>1037</v>
       </c>
       <c r="I234" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K234">
         <v>5733</v>
@@ -17245,7 +17255,7 @@
         <v>1037</v>
       </c>
       <c r="I235" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K235">
         <v>5706</v>
@@ -17298,10 +17308,10 @@
         <v>1037</v>
       </c>
       <c r="I236" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J236" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K236">
         <v>5611</v>
@@ -17354,10 +17364,10 @@
         <v>1037</v>
       </c>
       <c r="I237" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J237" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K237">
         <v>5430</v>
@@ -17410,7 +17420,7 @@
         <v>1037</v>
       </c>
       <c r="I238" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K238">
         <v>5417</v>
@@ -17463,7 +17473,7 @@
         <v>1037</v>
       </c>
       <c r="I239" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K239">
         <v>5319</v>
@@ -17516,10 +17526,10 @@
         <v>1037</v>
       </c>
       <c r="I240" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J240" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K240">
         <v>5187</v>
@@ -17572,10 +17582,10 @@
         <v>1037</v>
       </c>
       <c r="I241" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J241" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K241">
         <v>4886</v>
@@ -17628,10 +17638,10 @@
         <v>1037</v>
       </c>
       <c r="I242" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J242" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="K242">
         <v>4861</v>
@@ -17684,7 +17694,7 @@
         <v>1037</v>
       </c>
       <c r="I243" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K243">
         <v>4821</v>
@@ -17737,10 +17747,10 @@
         <v>5295</v>
       </c>
       <c r="I244" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J244" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="K244">
         <v>4717</v>
@@ -17793,7 +17803,7 @@
         <v>1037</v>
       </c>
       <c r="I245" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K245">
         <v>4533</v>
@@ -17849,10 +17859,10 @@
         <v>1037</v>
       </c>
       <c r="I246" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J246" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="K246">
         <v>4394</v>
@@ -17910,10 +17920,10 @@
         <v>5339</v>
       </c>
       <c r="I247" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J247" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="K247">
         <v>4365</v>
@@ -17966,10 +17976,10 @@
         <v>1037</v>
       </c>
       <c r="I248" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J248" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K248">
         <v>4260</v>
@@ -18025,10 +18035,10 @@
         <v>219486</v>
       </c>
       <c r="I249" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J249" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="K249">
         <v>4249</v>
@@ -18081,10 +18091,10 @@
         <v>1037</v>
       </c>
       <c r="I250" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J250" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K250">
         <v>4091</v>
@@ -18140,10 +18150,10 @@
         <v>155844</v>
       </c>
       <c r="I251" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J251" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="K251">
         <v>4084</v>
@@ -18196,10 +18206,10 @@
         <v>1037</v>
       </c>
       <c r="I252" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J252" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="K252">
         <v>4040</v>
@@ -18252,10 +18262,10 @@
         <v>262277</v>
       </c>
       <c r="I253" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J253" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="K253">
         <v>4000</v>
@@ -18308,10 +18318,10 @@
         <v>1037</v>
       </c>
       <c r="I254" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J254" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="K254">
         <v>3903</v>
@@ -18367,10 +18377,10 @@
         <v>1037</v>
       </c>
       <c r="I255" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J255" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K255">
         <v>3769</v>
@@ -18426,10 +18436,10 @@
         <v>1037</v>
       </c>
       <c r="I256" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J256" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="K256">
         <v>3677</v>
@@ -18485,7 +18495,7 @@
         <v>935</v>
       </c>
       <c r="I257" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J257" t="s">
         <v>604</v>
@@ -18544,10 +18554,10 @@
         <v>29711</v>
       </c>
       <c r="I258" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J258" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="K258">
         <v>3347</v>
@@ -18600,10 +18610,10 @@
         <v>1037</v>
       </c>
       <c r="I259" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J259" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K259">
         <v>3277</v>
@@ -18656,10 +18666,10 @@
         <v>1037</v>
       </c>
       <c r="I260" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J260" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="K260">
         <v>3270</v>
@@ -18724,7 +18734,7 @@
         <v>1037</v>
       </c>
       <c r="I261" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K261">
         <v>3153</v>
@@ -18777,10 +18787,10 @@
         <v>1037</v>
       </c>
       <c r="I262" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J262" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K262">
         <v>3149</v>
@@ -18833,7 +18843,7 @@
         <v>1037</v>
       </c>
       <c r="I263" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K263">
         <v>3123</v>
@@ -18886,10 +18896,10 @@
         <v>1037</v>
       </c>
       <c r="I264" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J264" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K264">
         <v>3092</v>
@@ -18933,7 +18943,7 @@
         <v>279</v>
       </c>
       <c r="E265" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="F265" t="s">
         <v>1037</v>
@@ -18942,10 +18952,10 @@
         <v>2621</v>
       </c>
       <c r="I265" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J265" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="K265">
         <v>3077</v>
@@ -18998,10 +19008,10 @@
         <v>1037</v>
       </c>
       <c r="I266" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J266" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K266">
         <v>2903</v>
@@ -19054,10 +19064,10 @@
         <v>25096</v>
       </c>
       <c r="I267" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J267" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="K267">
         <v>2839</v>
@@ -19113,10 +19123,10 @@
         <v>23013</v>
       </c>
       <c r="I268" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J268" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="K268">
         <v>2749</v>
@@ -19169,7 +19179,7 @@
         <v>1037</v>
       </c>
       <c r="I269" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K269">
         <v>2697</v>
@@ -19223,7 +19233,7 @@
         <v>10382205</v>
       </c>
       <c r="I270" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J270" t="s">
         <v>398</v>
@@ -19279,7 +19289,7 @@
         <v>1037</v>
       </c>
       <c r="I271" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K271">
         <v>2485</v>
@@ -19326,7 +19336,7 @@
         <v>774</v>
       </c>
       <c r="E272" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="F272" t="s">
         <v>1037</v>
@@ -19335,7 +19345,7 @@
         <v>11464</v>
       </c>
       <c r="I272" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="K272">
         <v>2471</v>
@@ -19391,7 +19401,7 @@
         <v>384653</v>
       </c>
       <c r="I273" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="K273">
         <v>2404</v>
@@ -19444,7 +19454,7 @@
         <v>1037</v>
       </c>
       <c r="I274" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K274">
         <v>2390</v>
@@ -19497,10 +19507,10 @@
         <v>1037</v>
       </c>
       <c r="I275" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J275" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K275">
         <v>2336</v>
@@ -19556,10 +19566,10 @@
         <v>1037</v>
       </c>
       <c r="I276" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J276" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K276">
         <v>2266</v>
@@ -19624,7 +19634,7 @@
         <v>1037</v>
       </c>
       <c r="I277" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K277">
         <v>2222</v>
@@ -19689,10 +19699,10 @@
         <v>1037</v>
       </c>
       <c r="I278" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J278" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K278">
         <v>2120</v>
@@ -19745,7 +19755,7 @@
         <v>1037</v>
       </c>
       <c r="I279" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K279">
         <v>2114</v>
@@ -19801,10 +19811,10 @@
         <v>1037</v>
       </c>
       <c r="I280" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J280" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="K280">
         <v>1946</v>
@@ -19857,10 +19867,10 @@
         <v>1037</v>
       </c>
       <c r="I281" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J281" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K281">
         <v>1932</v>
@@ -19919,7 +19929,7 @@
         <v>23665</v>
       </c>
       <c r="I282" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J282" t="s">
         <v>456</v>
@@ -19975,10 +19985,10 @@
         <v>1037</v>
       </c>
       <c r="I283" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J283" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K283">
         <v>1887</v>
@@ -20031,7 +20041,7 @@
         <v>1037</v>
       </c>
       <c r="I284" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K284">
         <v>1764</v>
@@ -20090,10 +20100,10 @@
         <v>22</v>
       </c>
       <c r="I285" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J285" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="K285">
         <v>1665</v>
@@ -20146,10 +20156,10 @@
         <v>1037</v>
       </c>
       <c r="I286" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J286" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="K286">
         <v>1664</v>
@@ -20202,7 +20212,7 @@
         <v>1037</v>
       </c>
       <c r="I287" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K287">
         <v>1583</v>
@@ -20255,7 +20265,7 @@
         <v>1037</v>
       </c>
       <c r="I288" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K288">
         <v>1502</v>
@@ -20311,7 +20321,7 @@
         <v>1037</v>
       </c>
       <c r="I289" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K289">
         <v>1502</v>
@@ -20367,7 +20377,7 @@
         <v>251</v>
       </c>
       <c r="I290" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="K290">
         <v>1463</v>
@@ -20420,10 +20430,10 @@
         <v>1037</v>
       </c>
       <c r="I291" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J291" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="K291">
         <v>1448</v>
@@ -20476,7 +20486,7 @@
         <v>1037</v>
       </c>
       <c r="I292" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K292">
         <v>1439</v>
@@ -20529,10 +20539,10 @@
         <v>1037</v>
       </c>
       <c r="I293" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J293" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="K293">
         <v>1429</v>
@@ -20585,10 +20595,10 @@
         <v>1037</v>
       </c>
       <c r="I294" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J294" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K294">
         <v>1391</v>
@@ -20641,10 +20651,10 @@
         <v>1037</v>
       </c>
       <c r="I295" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J295" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="K295">
         <v>1331</v>
@@ -20697,10 +20707,10 @@
         <v>1037</v>
       </c>
       <c r="I296" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J296" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K296">
         <v>1250</v>
@@ -20753,10 +20763,10 @@
         <v>1037</v>
       </c>
       <c r="I297" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J297" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K297">
         <v>1203</v>
@@ -20812,7 +20822,7 @@
         <v>14238</v>
       </c>
       <c r="I298" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="K298">
         <v>1184</v>
@@ -20865,10 +20875,10 @@
         <v>1037</v>
       </c>
       <c r="I299" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J299" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K299">
         <v>1160</v>
@@ -20921,10 +20931,10 @@
         <v>1037</v>
       </c>
       <c r="I300" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J300" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="K300">
         <v>1126</v>
@@ -20977,7 +20987,7 @@
         <v>1037</v>
       </c>
       <c r="I301" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K301">
         <v>1099</v>
@@ -21030,10 +21040,10 @@
         <v>1037</v>
       </c>
       <c r="I302" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J302" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K302">
         <v>953</v>
@@ -21086,10 +21096,10 @@
         <v>1037</v>
       </c>
       <c r="I303" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J303" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K303">
         <v>838</v>
@@ -21142,7 +21152,7 @@
         <v>1037</v>
       </c>
       <c r="I304" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K304">
         <v>831</v>
@@ -21198,10 +21208,10 @@
         <v>1037</v>
       </c>
       <c r="I305" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J305" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="K305">
         <v>830</v>
@@ -21254,10 +21264,10 @@
         <v>1037</v>
       </c>
       <c r="I306" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J306" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K306">
         <v>789</v>
@@ -21310,10 +21320,10 @@
         <v>1037</v>
       </c>
       <c r="I307" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J307" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K307">
         <v>782</v>
@@ -21369,7 +21379,7 @@
         <v>1037</v>
       </c>
       <c r="I308" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K308">
         <v>687</v>
@@ -21422,7 +21432,7 @@
         <v>1037</v>
       </c>
       <c r="I309" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K309">
         <v>687</v>
@@ -21475,7 +21485,7 @@
         <v>1037</v>
       </c>
       <c r="I310" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K310">
         <v>684</v>
@@ -21519,7 +21529,7 @@
         <v>554</v>
       </c>
       <c r="E311" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="F311" t="s">
         <v>1037</v>
@@ -21528,10 +21538,10 @@
         <v>48248</v>
       </c>
       <c r="I311" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J311" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="K311">
         <v>620</v>
@@ -21584,10 +21594,10 @@
         <v>1037</v>
       </c>
       <c r="I312" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J312" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="K312">
         <v>572</v>
@@ -21640,7 +21650,7 @@
         <v>1037</v>
       </c>
       <c r="I313" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K313">
         <v>466</v>
@@ -21705,7 +21715,7 @@
         <v>60</v>
       </c>
       <c r="I314" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="K314">
         <v>414</v>
@@ -21758,7 +21768,7 @@
         <v>1037</v>
       </c>
       <c r="I315" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K315">
         <v>388</v>
@@ -21811,7 +21821,7 @@
         <v>1037</v>
       </c>
       <c r="I316" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K316">
         <v>341</v>
@@ -21864,10 +21874,10 @@
         <v>1037</v>
       </c>
       <c r="I317" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J317" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K317">
         <v>311</v>
@@ -21920,7 +21930,7 @@
         <v>1037</v>
       </c>
       <c r="I318" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K318">
         <v>301</v>
@@ -21976,7 +21986,7 @@
         <v>78423</v>
       </c>
       <c r="I319" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="K319">
         <v>292</v>
@@ -22020,7 +22030,7 @@
         <v>170</v>
       </c>
       <c r="E320" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="F320" t="s">
         <v>1037</v>
@@ -22029,10 +22039,10 @@
         <v>500</v>
       </c>
       <c r="I320" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J320" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="K320">
         <v>289</v>
@@ -22088,10 +22098,10 @@
         <v>1037</v>
       </c>
       <c r="I321" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J321" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K321">
         <v>272</v>
@@ -22144,10 +22154,10 @@
         <v>1037</v>
       </c>
       <c r="I322" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J322" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K322">
         <v>270</v>
@@ -22200,10 +22210,10 @@
         <v>1037</v>
       </c>
       <c r="I323" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J323" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K323">
         <v>260</v>
@@ -22256,10 +22266,10 @@
         <v>1037</v>
       </c>
       <c r="I324" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J324" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K324">
         <v>248</v>
@@ -22312,7 +22322,7 @@
         <v>1037</v>
       </c>
       <c r="I325" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K325">
         <v>248</v>
@@ -22368,7 +22378,7 @@
         <v>1037</v>
       </c>
       <c r="I326" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K326">
         <v>248</v>
@@ -22421,10 +22431,10 @@
         <v>6347010</v>
       </c>
       <c r="I327" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J327" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="K327">
         <v>236</v>
@@ -22480,10 +22490,10 @@
         <v>1037</v>
       </c>
       <c r="I328" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J328" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="K328">
         <v>231</v>
@@ -22536,7 +22546,7 @@
         <v>1037</v>
       </c>
       <c r="I329" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K329">
         <v>231</v>
@@ -22592,7 +22602,7 @@
         <v>1037</v>
       </c>
       <c r="I330" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K330">
         <v>230</v>
@@ -22645,7 +22655,7 @@
         <v>1037</v>
       </c>
       <c r="I331" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K331">
         <v>218</v>
@@ -22698,10 +22708,10 @@
         <v>1037</v>
       </c>
       <c r="I332" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J332" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K332">
         <v>210</v>
@@ -22754,10 +22764,10 @@
         <v>13134</v>
       </c>
       <c r="I333" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J333" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="K333">
         <v>177</v>
@@ -22813,10 +22823,10 @@
         <v>1037</v>
       </c>
       <c r="I334" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J334" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K334">
         <v>160</v>
@@ -22869,7 +22879,7 @@
         <v>1037</v>
       </c>
       <c r="I335" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K335">
         <v>146</v>
@@ -22922,7 +22932,7 @@
         <v>1037</v>
       </c>
       <c r="I336" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="K336">
         <v>137</v>
@@ -22975,10 +22985,10 @@
         <v>1037</v>
       </c>
       <c r="I337" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J337" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K337">
         <v>114</v>
@@ -23031,10 +23041,10 @@
         <v>1037</v>
       </c>
       <c r="I338" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J338" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="K338">
         <v>103</v>
@@ -23087,10 +23097,10 @@
         <v>1037</v>
       </c>
       <c r="I339" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J339" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="L339" t="s">
         <v>292</v>
@@ -23140,10 +23150,10 @@
         <v>1037</v>
       </c>
       <c r="I340" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J340" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="L340" t="s">
         <v>404</v>
@@ -23193,10 +23203,10 @@
         <v>1037</v>
       </c>
       <c r="I341" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J341" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="L341" t="s">
         <v>63</v>
@@ -23246,10 +23256,10 @@
         <v>1037</v>
       </c>
       <c r="I342" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J342" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="L342" t="s">
         <v>462</v>
@@ -23299,10 +23309,10 @@
         <v>1037</v>
       </c>
       <c r="I343" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J343" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="L343" t="s">
         <v>219</v>
@@ -23352,10 +23362,10 @@
         <v>1037</v>
       </c>
       <c r="I344" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J344" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="L344" t="s">
         <v>640</v>
@@ -23417,10 +23427,10 @@
         <v>1037</v>
       </c>
       <c r="I345" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J345" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="L345" t="s">
         <v>647</v>
@@ -23473,10 +23483,10 @@
         <v>1037</v>
       </c>
       <c r="I346" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J346" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="L346" t="s">
         <v>685</v>
@@ -23529,10 +23539,10 @@
         <v>1037</v>
       </c>
       <c r="I347" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J347" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="L347" t="s">
         <v>894</v>
@@ -23582,10 +23592,10 @@
         <v>1037</v>
       </c>
       <c r="I348" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J348" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="L348" t="s">
         <v>493</v>
@@ -23635,10 +23645,10 @@
         <v>1037</v>
       </c>
       <c r="I349" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J349" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="L349" t="s">
         <v>496</v>
@@ -23688,10 +23698,10 @@
         <v>1037</v>
       </c>
       <c r="I350" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J350" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="L350" t="s">
         <v>498</v>
@@ -23741,10 +23751,10 @@
         <v>1037</v>
       </c>
       <c r="I351" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J351" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="L351" t="s">
         <v>517</v>
@@ -23794,10 +23804,10 @@
         <v>1037</v>
       </c>
       <c r="I352" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J352" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="L352" t="s">
         <v>534</v>
@@ -23847,10 +23857,10 @@
         <v>1037</v>
       </c>
       <c r="I353" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J353" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="L353" t="s">
         <v>587</v>
@@ -23900,10 +23910,10 @@
         <v>1037</v>
       </c>
       <c r="I354" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J354" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="L354" t="s">
         <v>602</v>
@@ -23953,10 +23963,10 @@
         <v>1037</v>
       </c>
       <c r="I355" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J355" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="L355" t="s">
         <v>615</v>
@@ -24006,10 +24016,10 @@
         <v>1037</v>
       </c>
       <c r="I356" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J356" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="L356" t="s">
         <v>623</v>
@@ -24059,10 +24069,10 @@
         <v>1037</v>
       </c>
       <c r="I357" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J357" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="L357" t="s">
         <v>148</v>
@@ -24115,10 +24125,10 @@
         <v>1037</v>
       </c>
       <c r="I358" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J358" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="L358" t="s">
         <v>658</v>
@@ -24171,10 +24181,10 @@
         <v>1037</v>
       </c>
       <c r="I359" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J359" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="L359" t="s">
         <v>670</v>
@@ -24224,10 +24234,10 @@
         <v>1037</v>
       </c>
       <c r="I360" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J360" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="L360" t="s">
         <v>945</v>
@@ -24277,10 +24287,10 @@
         <v>1037</v>
       </c>
       <c r="I361" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J361" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="L361" t="s">
         <v>414</v>
@@ -24330,10 +24340,10 @@
         <v>1037</v>
       </c>
       <c r="I362" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J362" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="L362" t="s">
         <v>36</v>
@@ -24383,7 +24393,7 @@
         <v>1037</v>
       </c>
       <c r="I363" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="L363" t="s">
         <v>858</v>
@@ -24436,7 +24446,7 @@
         <v>1037</v>
       </c>
       <c r="I364" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="L364" t="s">
         <v>613</v>
@@ -24486,7 +24496,7 @@
         <v>1037</v>
       </c>
       <c r="I365" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="L365" t="s">
         <v>763</v>
@@ -24539,7 +24549,7 @@
         <v>1037</v>
       </c>
       <c r="I366" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="L366" t="s">
         <v>853</v>
@@ -24592,7 +24602,7 @@
         <v>1037</v>
       </c>
       <c r="I367" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="L367" t="s">
         <v>693</v>
@@ -24645,7 +24655,7 @@
         <v>1037</v>
       </c>
       <c r="I368" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="L368" t="s">
         <v>731</v>
@@ -24695,10 +24705,10 @@
         <v>1037</v>
       </c>
       <c r="I369" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J369" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="L369" t="s">
         <v>806</v>
@@ -24748,10 +24758,10 @@
         <v>1037</v>
       </c>
       <c r="I370" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="J370" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="L370" t="s">
         <v>668</v>
@@ -24813,7 +24823,7 @@
         <v>1037</v>
       </c>
       <c r="I371" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="L371" t="s">
         <v>190</v>
@@ -24863,7 +24873,7 @@
         <v>1037</v>
       </c>
       <c r="I372" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="L372" t="s">
         <v>54</v>
@@ -24913,7 +24923,7 @@
         <v>1037</v>
       </c>
       <c r="I373" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="L373" t="s">
         <v>861</v>
@@ -24966,7 +24976,7 @@
         <v>1037</v>
       </c>
       <c r="I374" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="L374" t="s">
         <v>553</v>
@@ -25016,10 +25026,10 @@
         <v>2155</v>
       </c>
       <c r="I375" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J375" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="L375" t="s">
         <v>598</v>
@@ -25063,7 +25073,7 @@
         <v>67</v>
       </c>
       <c r="E376" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="F376" t="s">
         <v>1037</v>
@@ -25072,10 +25082,10 @@
         <v>4245</v>
       </c>
       <c r="I376" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J376" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="L376" t="s">
         <v>68</v>
@@ -25128,10 +25138,10 @@
         <v>2</v>
       </c>
       <c r="I377" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="J377" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="L377" t="s">
         <v>76</v>
@@ -25181,10 +25191,10 @@
         <v>3</v>
       </c>
       <c r="I378" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J378" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="L378" t="s">
         <v>247</v>

</xml_diff>